<commit_message>
renew sprintReport and correct some label errors.
</commit_message>
<xml_diff>
--- a/Team01Report.xlsx
+++ b/Team01Report.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10808" tabRatio="477" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10808" tabRatio="477" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="213">
   <si>
     <t>Initials</t>
   </si>
@@ -373,39 +373,18 @@
     <t>cl</t>
   </si>
   <si>
-    <t>T03.01</t>
-  </si>
-  <si>
-    <t>T03.02</t>
-  </si>
-  <si>
-    <t>T03.03</t>
-  </si>
-  <si>
-    <t>T04.01</t>
-  </si>
-  <si>
     <t>Store marriage date</t>
   </si>
   <si>
-    <t>T04.02</t>
-  </si>
-  <si>
     <t>Store two birth dates</t>
   </si>
   <si>
-    <t>T04.03</t>
-  </si>
-  <si>
     <t>Compare birth and marriage date, and the year of age 14</t>
   </si>
   <si>
     <t>fl</t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
     <t>Keep doing:</t>
   </si>
   <si>
@@ -653,6 +632,48 @@
   </si>
   <si>
     <t>URL: https://github.com/cliang6/CS_555_GEDCOM_Project</t>
+  </si>
+  <si>
+    <t>T09.01</t>
+  </si>
+  <si>
+    <t>T09.02</t>
+  </si>
+  <si>
+    <t>T09.03</t>
+  </si>
+  <si>
+    <t>T10.01</t>
+  </si>
+  <si>
+    <t>T10.02</t>
+  </si>
+  <si>
+    <t>T10.03</t>
+  </si>
+  <si>
+    <t>T17.01</t>
+  </si>
+  <si>
+    <t>T17.02</t>
+  </si>
+  <si>
+    <t>T17.03</t>
+  </si>
+  <si>
+    <t>T18.01</t>
+  </si>
+  <si>
+    <t>T18.02</t>
+  </si>
+  <si>
+    <t>T18.03</t>
+  </si>
+  <si>
+    <t>Store birth date of children</t>
+  </si>
+  <si>
+    <t>Store death date of parent</t>
   </si>
 </sst>
 </file>
@@ -663,7 +684,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -682,6 +703,24 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF7030A0"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
@@ -712,7 +751,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -737,6 +776,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2002,10 +2044,10 @@
         <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="F9" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -2027,8 +2069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4"/>
@@ -2706,14 +2748,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I83"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4"/>
   <cols>
     <col min="1" max="1" width="7.64453125" customWidth="1"/>
-    <col min="2" max="2" width="24.46875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.46875" style="2" customWidth="1"/>
     <col min="3" max="3" width="6.64453125" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
@@ -2752,7 +2794,7 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" t="s">
+      <c r="A2" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2771,8 +2813,11 @@
         <v>60</v>
       </c>
     </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="14"/>
+    </row>
     <row r="4" spans="1:9">
-      <c r="A4" t="s">
+      <c r="A4" s="14" t="s">
         <v>99</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -2783,7 +2828,7 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" t="s">
+      <c r="A5" s="14" t="s">
         <v>101</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -2793,8 +2838,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="24.75">
-      <c r="A6" t="s">
+    <row r="6" spans="1:9">
+      <c r="A6" s="14" t="s">
         <v>103</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -2804,8 +2849,11 @@
         <v>5</v>
       </c>
     </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="14"/>
+    </row>
     <row r="8" spans="1:9">
-      <c r="A8" t="s">
+      <c r="A8" s="14" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -2824,8 +2872,11 @@
         <v>60</v>
       </c>
     </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="14"/>
+    </row>
     <row r="10" spans="1:9" ht="24.75">
-      <c r="A10" t="s">
+      <c r="A10" s="14" t="s">
         <v>105</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -2836,7 +2887,7 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" t="s">
+      <c r="A11" s="14" t="s">
         <v>107</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -2847,7 +2898,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="24.75">
-      <c r="A12" t="s">
+      <c r="A12" s="14" t="s">
         <v>109</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -2857,12 +2908,15 @@
         <v>5</v>
       </c>
     </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="14"/>
+    </row>
     <row r="14" spans="1:9">
-      <c r="A14" t="s">
-        <v>32</v>
+      <c r="A14" s="15" t="s">
+        <v>44</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
         <v>111</v>
@@ -2877,31 +2931,34 @@
         <v>60</v>
       </c>
     </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="15"/>
+    </row>
     <row r="16" spans="1:9">
-      <c r="A16" t="s">
-        <v>112</v>
+      <c r="A16" s="15" t="s">
+        <v>199</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>100</v>
+        <v>211</v>
       </c>
       <c r="C16" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" t="s">
-        <v>113</v>
+      <c r="A17" s="15" t="s">
+        <v>200</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>102</v>
+        <v>212</v>
       </c>
       <c r="C17" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="24.75">
-      <c r="A18" t="s">
-        <v>114</v>
+    <row r="18" spans="1:6">
+      <c r="A18" s="15" t="s">
+        <v>201</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>104</v>
@@ -2910,9 +2967,12 @@
         <v>111</v>
       </c>
     </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="15"/>
+    </row>
     <row r="20" spans="1:6">
-      <c r="A20" t="s">
-        <v>34</v>
+      <c r="A20" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="B20" t="s">
         <v>35</v>
@@ -2930,51 +2990,54 @@
         <v>60</v>
       </c>
     </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="15"/>
+    </row>
     <row r="22" spans="1:6">
-      <c r="A22" t="s">
-        <v>115</v>
+      <c r="A22" s="15" t="s">
+        <v>202</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C22" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" t="s">
-        <v>117</v>
+      <c r="A23" s="15" t="s">
+        <v>203</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C23" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="24.75">
-      <c r="A24" t="s">
-        <v>119</v>
+      <c r="A24" s="15" t="s">
+        <v>204</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C24" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" t="s">
-        <v>32</v>
+      <c r="A26" s="16" t="s">
+        <v>60</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C26" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D26" t="s">
-        <v>122</v>
+        <v>29</v>
       </c>
       <c r="E26">
         <v>150</v>
@@ -2983,51 +3046,48 @@
         <v>60</v>
       </c>
     </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="16"/>
+    </row>
     <row r="28" spans="1:6">
-      <c r="A28" t="s">
-        <v>112</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>100</v>
+      <c r="A28" s="16" t="s">
+        <v>205</v>
       </c>
       <c r="C28" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" t="s">
-        <v>113</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>102</v>
+      <c r="A29" s="16" t="s">
+        <v>206</v>
       </c>
       <c r="C29" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="24.75">
-      <c r="A30" t="s">
-        <v>114</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>104</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="16" t="s">
+        <v>207</v>
       </c>
       <c r="C30" t="s">
-        <v>121</v>
-      </c>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="16"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" t="s">
-        <v>32</v>
+      <c r="A32" s="16" t="s">
+        <v>62</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C32" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D32" t="s">
-        <v>122</v>
+        <v>29</v>
       </c>
       <c r="E32">
         <v>150</v>
@@ -3036,37 +3096,31 @@
         <v>60</v>
       </c>
     </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="16"/>
+    </row>
     <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>112</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>100</v>
+      <c r="A34" s="16" t="s">
+        <v>208</v>
       </c>
       <c r="C34" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>113</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>102</v>
+      <c r="A35" s="16" t="s">
+        <v>209</v>
       </c>
       <c r="C35" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="24.75">
-      <c r="A36" t="s">
-        <v>114</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>104</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="16" t="s">
+        <v>210</v>
       </c>
       <c r="C36" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="77" spans="2:2">
@@ -3077,18 +3131,18 @@
     </row>
     <row r="79" spans="2:2">
       <c r="B79" s="3" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="83" spans="2:2">
       <c r="B83" s="3" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3232,8 +3286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4"/>
@@ -3250,7 +3304,7 @@
         <v>23</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30">
@@ -3261,7 +3315,7 @@
         <v>27</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15">
@@ -3272,7 +3326,7 @@
         <v>31</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15">
@@ -3283,7 +3337,7 @@
         <v>41</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30">
@@ -3294,7 +3348,7 @@
         <v>43</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15">
@@ -3305,7 +3359,7 @@
         <v>53</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15">
@@ -3316,7 +3370,7 @@
         <v>55</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="45">
@@ -3327,7 +3381,7 @@
         <v>65</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30">
@@ -3338,7 +3392,7 @@
         <v>67</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30">
@@ -3349,7 +3403,7 @@
         <v>33</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30">
@@ -3360,7 +3414,7 @@
         <v>35</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30">
@@ -3371,7 +3425,7 @@
         <v>45</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="45">
@@ -3382,7 +3436,7 @@
         <v>47</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="60">
@@ -3393,7 +3447,7 @@
         <v>57</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="30">
@@ -3404,7 +3458,7 @@
         <v>59</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15">
@@ -3415,7 +3469,7 @@
         <v>69</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30">
@@ -3426,7 +3480,7 @@
         <v>71</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15">
@@ -3437,7 +3491,7 @@
         <v>37</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15">
@@ -3448,7 +3502,7 @@
         <v>39</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15">
@@ -3459,7 +3513,7 @@
         <v>49</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="30">
@@ -3470,7 +3524,7 @@
         <v>51</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30">
@@ -3481,7 +3535,7 @@
         <v>61</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="30">
@@ -3492,7 +3546,7 @@
         <v>63</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30">
@@ -3503,7 +3557,7 @@
         <v>73</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="45">
@@ -3514,205 +3568,205 @@
         <v>75</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="30">
       <c r="A26" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B26" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="105">
       <c r="A27" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B27" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15">
       <c r="A28" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B28" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="30">
       <c r="A29" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B29" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15">
       <c r="A30" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B30" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15">
       <c r="A31" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B31" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="30">
       <c r="A32" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B32" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15">
       <c r="A33" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B33" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="30">
       <c r="A34" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B34" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="30">
       <c r="A35" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B35" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="30">
       <c r="A36" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="B36" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="30">
       <c r="A37" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B37" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="30">
       <c r="A38" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="B38" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="30">
       <c r="A39" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B39" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="30">
       <c r="A40" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="B40" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="30">
       <c r="A41" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="B41" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="30">
       <c r="A42" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B42" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="30">
       <c r="A43" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="B43" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>